<commit_message>
Add status to demonstrate DEFAULT VALUE feature
</commit_message>
<xml_diff>
--- a/src/ProjectAdministration.xlsx
+++ b/src/ProjectAdministration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\project-administration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\ampersand-tarski\project-administration\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BB983B-A216-45CE-BC53-D56985C62715}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A011F0-5CD7-4089-8C79-9B35E12222DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="3510" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>Project</t>
   </si>
@@ -712,22 +714,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -750,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -773,7 +775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -797,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
@@ -821,13 +823,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>51</v>
       </c>
@@ -838,12 +843,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>53</v>
@@ -853,12 +861,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>52</v>
@@ -872,7 +883,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>90</v>
       </c>
@@ -896,12 +907,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>91</v>
       </c>
@@ -910,7 +921,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -920,7 +931,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
@@ -928,7 +939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -936,7 +947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -944,7 +955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -952,7 +963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -960,7 +971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>86</v>
       </c>
@@ -968,7 +979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>86</v>
       </c>
@@ -976,7 +987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
@@ -984,7 +995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
@@ -992,7 +1003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>87</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -1008,7 +1019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>90</v>
       </c>
@@ -1016,7 +1027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>90</v>
       </c>
@@ -1034,20 +1045,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17" style="2" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +1076,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1083,7 +1094,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1101,7 +1112,7 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1127,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1131,7 +1142,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1149,7 +1160,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1175,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1179,7 +1190,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1194,7 +1205,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1209,7 +1220,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1235,7 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1239,7 +1250,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1254,7 +1265,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Add default population for worksWith
</commit_message>
<xml_diff>
--- a/src/ProjectAdministration.xlsx
+++ b/src/ProjectAdministration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\ampersand-tarski\project-administration\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A011F0-5CD7-4089-8C79-9B35E12222DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F39260D-979B-43E2-B148-C4571574C416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>Project</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>[Members]</t>
+  </si>
+  <si>
+    <t>workswith</t>
   </si>
 </sst>
 </file>
@@ -714,22 +717,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -752,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -775,7 +778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -799,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
@@ -823,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
@@ -843,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -861,7 +864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
@@ -883,7 +886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>90</v>
       </c>
@@ -907,12 +910,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>91</v>
       </c>
@@ -921,7 +924,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -931,7 +934,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
@@ -939,7 +942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -947,7 +950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -955,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -963,7 +966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -971,7 +974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>86</v>
       </c>
@@ -979,7 +982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>86</v>
       </c>
@@ -987,7 +990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
@@ -995,7 +998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>87</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>90</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>90</v>
       </c>
@@ -1043,22 +1046,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17" style="2" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -1074,9 +1077,14 @@
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1092,9 +1100,14 @@
       <c r="E2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1110,9 +1123,14 @@
       <c r="E3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1125,9 +1143,11 @@
       <c r="E4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1140,9 +1160,11 @@
       <c r="E5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1160,7 +1182,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1175,7 +1197,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1212,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1205,7 +1227,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -1220,7 +1242,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1235,7 +1257,7 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1272,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1265,7 +1287,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Multi value excel import sheet use case
</commit_message>
<xml_diff>
--- a/src/ProjectAdministration.xlsx
+++ b/src/ProjectAdministration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\ampersand-tarski\project-administration\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F39260D-979B-43E2-B148-C4571574C416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEEB4CA-899E-4DDD-8523-E812CDB764AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29010" yWindow="0" windowWidth="28590" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>Project</t>
   </si>
@@ -306,10 +306,22 @@
     <t>1970_13</t>
   </si>
   <si>
-    <t>[Members]</t>
-  </si>
-  <si>
     <t>workswith</t>
+  </si>
+  <si>
+    <t>[Person,]</t>
+  </si>
+  <si>
+    <t>p10001,p10002,p10003</t>
+  </si>
+  <si>
+    <t>p10001,p10003,p10004,p10005</t>
+  </si>
+  <si>
+    <t>p10002,p10003,p10005</t>
+  </si>
+  <si>
+    <t>p10006,p10009,p10010</t>
   </si>
 </sst>
 </file>
@@ -715,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,9 +742,10 @@
     <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -754,8 +767,11 @@
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -777,8 +793,11 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -801,8 +820,11 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
@@ -825,8 +847,11 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
@@ -845,8 +870,11 @@
       <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -864,7 +892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
@@ -886,7 +914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>90</v>
       </c>
@@ -909,22 +937,23 @@
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>91</v>
-      </c>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -934,7 +963,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
@@ -942,7 +971,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -950,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -958,7 +987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -966,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -1048,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,6 +1088,8 @@
     <col min="3" max="3" width="17" style="2" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1078,10 +1109,10 @@
         <v>28</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix .xlsx file, add [ and ] in cell A10
</commit_message>
<xml_diff>
--- a/src/ProjectAdministration.xlsx
+++ b/src/ProjectAdministration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\ampersand-tarski\project-administration\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\han\git\Ampersand\Project-administration\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEEB4CA-899E-4DDD-8523-E812CDB764AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7086A6B-AD1F-4F17-B6CE-6EFEC4A54BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="0" windowWidth="28590" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="2295" windowWidth="22530" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="98">
   <si>
     <t>Project</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>p10006,p10009,p10010</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -378,13 +381,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -407,9 +407,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -447,9 +447,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,26 +482,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,26 +517,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -730,23 +696,23 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -758,7 +724,7 @@
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -772,7 +738,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -784,10 +750,10 @@
       <c r="D2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -798,22 +764,22 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>41639</v>
       </c>
-      <c r="F3" s="5" t="str">
+      <c r="F3" t="str">
         <f>A3</f>
         <v>2013_01</v>
       </c>
@@ -824,147 +790,142 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>41685</v>
       </c>
-      <c r="F4" s="5" t="str">
+      <c r="F4" t="str">
         <f>A4</f>
         <v>2014_01</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>41835</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="5" t="str">
+      <c r="F7" t="str">
         <f>A7</f>
         <v>2014_05</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>25675</v>
       </c>
-      <c r="F8" s="5" t="str">
+      <c r="F8" t="str">
         <f>A8</f>
         <v>1970_13</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>85</v>
       </c>
       <c r="B12" t="s">
@@ -972,7 +933,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>85</v>
       </c>
       <c r="B13" t="s">
@@ -980,7 +941,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>85</v>
       </c>
       <c r="B14" t="s">
@@ -988,15 +949,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>86</v>
       </c>
       <c r="B16" t="s">
@@ -1004,7 +965,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>86</v>
       </c>
       <c r="B17" t="s">
@@ -1012,7 +973,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>86</v>
       </c>
       <c r="B18" t="s">
@@ -1020,15 +981,15 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
       <c r="B20" t="s">
@@ -1036,7 +997,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
         <v>87</v>
       </c>
       <c r="B21" t="s">
@@ -1044,15 +1005,15 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
       <c r="B23" t="s">
@@ -1060,7 +1021,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
         <v>90</v>
       </c>
       <c r="B24" t="s">
@@ -1084,8 +1045,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -1093,7 +1053,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1108,15 +1068,15 @@
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1131,207 +1091,207 @@
       <c r="E2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>